<commit_message>
replace some labels that were renamed between different versions of argument graphs
</commit_message>
<xml_diff>
--- a/data/external/ethikchat_data-main/mensateria_survey_2/processed/curated/mensateria_survey_2_refai_curated_dialogues.xlsx
+++ b/data/external/ethikchat_data-main/mensateria_survey_2/processed/curated/mensateria_survey_2_refai_curated_dialogues.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="542">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -946,9 +946,6 @@
     <t>['CONSENT']</t>
   </si>
   <si>
-    <t>['Z.P2-1']</t>
-  </si>
-  <si>
     <t>['Z.P5']</t>
   </si>
   <si>
@@ -1009,9 +1006,6 @@
     <t>['Z.K1-1-1-1']</t>
   </si>
   <si>
-    <t>['Z.P2-1-1']</t>
-  </si>
-  <si>
     <t>['intro_23', 'Z.K3-1', 'intro_4', 'z_trans_12', 'Z.K4']</t>
   </si>
   <si>
@@ -1055,9 +1049,6 @@
   </si>
   <si>
     <t>['intro_25', 'Z.P1', 'intro_48', 'Z.P1-2']</t>
-  </si>
-  <si>
-    <t>['Z.P3-4']</t>
   </si>
   <si>
     <t>['Z.P2', 'Z.P1']</t>
@@ -2055,7 +2046,7 @@
         <v>277</v>
       </c>
       <c r="G2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2078,7 +2069,7 @@
         <v>278</v>
       </c>
       <c r="G3" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2101,7 +2092,7 @@
         <v>277</v>
       </c>
       <c r="G4" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2124,7 +2115,7 @@
         <v>279</v>
       </c>
       <c r="G5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2147,7 +2138,7 @@
         <v>280</v>
       </c>
       <c r="G6" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2170,7 +2161,7 @@
         <v>280</v>
       </c>
       <c r="G7" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2193,7 +2184,7 @@
         <v>281</v>
       </c>
       <c r="G8" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -2216,7 +2207,7 @@
         <v>282</v>
       </c>
       <c r="G9" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2239,7 +2230,7 @@
         <v>283</v>
       </c>
       <c r="G10" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -2262,7 +2253,7 @@
         <v>283</v>
       </c>
       <c r="G11" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2285,7 +2276,7 @@
         <v>277</v>
       </c>
       <c r="G12" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2308,7 +2299,7 @@
         <v>277</v>
       </c>
       <c r="G13" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2331,7 +2322,7 @@
         <v>284</v>
       </c>
       <c r="G14" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2354,7 +2345,7 @@
         <v>285</v>
       </c>
       <c r="G15" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -2377,7 +2368,7 @@
         <v>286</v>
       </c>
       <c r="G16" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2400,7 +2391,7 @@
         <v>277</v>
       </c>
       <c r="G17" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -2423,7 +2414,7 @@
         <v>287</v>
       </c>
       <c r="G18" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -2446,7 +2437,7 @@
         <v>288</v>
       </c>
       <c r="G19" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -2469,7 +2460,7 @@
         <v>289</v>
       </c>
       <c r="G20" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2492,7 +2483,7 @@
         <v>290</v>
       </c>
       <c r="G21" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2515,7 +2506,7 @@
         <v>291</v>
       </c>
       <c r="G22" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -2538,7 +2529,7 @@
         <v>292</v>
       </c>
       <c r="G23" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2561,7 +2552,7 @@
         <v>293</v>
       </c>
       <c r="G24" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -2584,7 +2575,7 @@
         <v>293</v>
       </c>
       <c r="G25" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -2607,7 +2598,7 @@
         <v>277</v>
       </c>
       <c r="G26" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -2630,7 +2621,7 @@
         <v>294</v>
       </c>
       <c r="G27" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -2653,7 +2644,7 @@
         <v>295</v>
       </c>
       <c r="G28" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -2676,7 +2667,7 @@
         <v>287</v>
       </c>
       <c r="G29" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -2699,7 +2690,7 @@
         <v>296</v>
       </c>
       <c r="G30" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -2722,7 +2713,7 @@
         <v>293</v>
       </c>
       <c r="G31" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2745,7 +2736,7 @@
         <v>293</v>
       </c>
       <c r="G32" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -2768,7 +2759,7 @@
         <v>291</v>
       </c>
       <c r="G33" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -2791,7 +2782,7 @@
         <v>295</v>
       </c>
       <c r="G34" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -2814,7 +2805,7 @@
         <v>295</v>
       </c>
       <c r="G35" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -2837,7 +2828,7 @@
         <v>290</v>
       </c>
       <c r="G36" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2860,7 +2851,7 @@
         <v>297</v>
       </c>
       <c r="G37" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -2883,7 +2874,7 @@
         <v>298</v>
       </c>
       <c r="G38" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -2906,7 +2897,7 @@
         <v>299</v>
       </c>
       <c r="G39" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -2929,7 +2920,7 @@
         <v>293</v>
       </c>
       <c r="G40" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -2952,7 +2943,7 @@
         <v>293</v>
       </c>
       <c r="G41" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -2975,7 +2966,7 @@
         <v>277</v>
       </c>
       <c r="G42" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2998,7 +2989,7 @@
         <v>300</v>
       </c>
       <c r="G43" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -3021,7 +3012,7 @@
         <v>301</v>
       </c>
       <c r="G44" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -3044,7 +3035,7 @@
         <v>302</v>
       </c>
       <c r="G45" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -3067,7 +3058,7 @@
         <v>302</v>
       </c>
       <c r="G46" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -3090,7 +3081,7 @@
         <v>295</v>
       </c>
       <c r="G47" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -3113,7 +3104,7 @@
         <v>290</v>
       </c>
       <c r="G48" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -3136,7 +3127,7 @@
         <v>291</v>
       </c>
       <c r="G49" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -3159,7 +3150,7 @@
         <v>291</v>
       </c>
       <c r="G50" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -3182,7 +3173,7 @@
         <v>290</v>
       </c>
       <c r="G51" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -3205,7 +3196,7 @@
         <v>295</v>
       </c>
       <c r="G52" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -3228,7 +3219,7 @@
         <v>287</v>
       </c>
       <c r="G53" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -3251,7 +3242,7 @@
         <v>287</v>
       </c>
       <c r="G54" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -3274,7 +3265,7 @@
         <v>303</v>
       </c>
       <c r="G55" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -3297,7 +3288,7 @@
         <v>304</v>
       </c>
       <c r="G56" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -3320,7 +3311,7 @@
         <v>305</v>
       </c>
       <c r="G57" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -3343,7 +3334,7 @@
         <v>306</v>
       </c>
       <c r="G58" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -3366,7 +3357,7 @@
         <v>277</v>
       </c>
       <c r="G59" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -3389,7 +3380,7 @@
         <v>290</v>
       </c>
       <c r="G60" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -3412,7 +3403,7 @@
         <v>302</v>
       </c>
       <c r="G61" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -3435,7 +3426,7 @@
         <v>290</v>
       </c>
       <c r="G62" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -3458,7 +3449,7 @@
         <v>291</v>
       </c>
       <c r="G63" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -3481,7 +3472,7 @@
         <v>295</v>
       </c>
       <c r="G64" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -3504,7 +3495,7 @@
         <v>307</v>
       </c>
       <c r="G65" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -3527,7 +3518,7 @@
         <v>277</v>
       </c>
       <c r="G66" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -3550,7 +3541,7 @@
         <v>308</v>
       </c>
       <c r="G67" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -3573,7 +3564,7 @@
         <v>309</v>
       </c>
       <c r="G68" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -3596,7 +3587,7 @@
         <v>290</v>
       </c>
       <c r="G69" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -3616,10 +3607,10 @@
         <v>103</v>
       </c>
       <c r="F70" t="s">
-        <v>310</v>
+        <v>280</v>
       </c>
       <c r="G70" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -3642,7 +3633,7 @@
         <v>277</v>
       </c>
       <c r="G71" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -3665,7 +3656,7 @@
         <v>293</v>
       </c>
       <c r="G72" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -3688,7 +3679,7 @@
         <v>293</v>
       </c>
       <c r="G73" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -3708,10 +3699,10 @@
         <v>106</v>
       </c>
       <c r="F74" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G74" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -3734,7 +3725,7 @@
         <v>284</v>
       </c>
       <c r="G75" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -3754,10 +3745,10 @@
         <v>108</v>
       </c>
       <c r="F76" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G76" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -3780,7 +3771,7 @@
         <v>280</v>
       </c>
       <c r="G77" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -3803,7 +3794,7 @@
         <v>309</v>
       </c>
       <c r="G78" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -3826,7 +3817,7 @@
         <v>280</v>
       </c>
       <c r="G79" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -3846,10 +3837,10 @@
         <v>112</v>
       </c>
       <c r="F80" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G80" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -3869,10 +3860,10 @@
         <v>113</v>
       </c>
       <c r="F81" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G81" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -3892,10 +3883,10 @@
         <v>114</v>
       </c>
       <c r="F82" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G82" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -3918,7 +3909,7 @@
         <v>295</v>
       </c>
       <c r="G83" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -3941,7 +3932,7 @@
         <v>283</v>
       </c>
       <c r="G84" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -3961,10 +3952,10 @@
         <v>116</v>
       </c>
       <c r="F85" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G85" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -3987,7 +3978,7 @@
         <v>290</v>
       </c>
       <c r="G86" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -4010,7 +4001,7 @@
         <v>295</v>
       </c>
       <c r="G87" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -4033,7 +4024,7 @@
         <v>290</v>
       </c>
       <c r="G88" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -4056,7 +4047,7 @@
         <v>277</v>
       </c>
       <c r="G89" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -4079,7 +4070,7 @@
         <v>290</v>
       </c>
       <c r="G90" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -4102,7 +4093,7 @@
         <v>302</v>
       </c>
       <c r="G91" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -4125,7 +4116,7 @@
         <v>302</v>
       </c>
       <c r="G92" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -4145,10 +4136,10 @@
         <v>122</v>
       </c>
       <c r="F93" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G93" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -4168,10 +4159,10 @@
         <v>123</v>
       </c>
       <c r="F94" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G94" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -4194,7 +4185,7 @@
         <v>284</v>
       </c>
       <c r="G95" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -4217,7 +4208,7 @@
         <v>277</v>
       </c>
       <c r="G96" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -4237,10 +4228,10 @@
         <v>126</v>
       </c>
       <c r="F97" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G97" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -4260,10 +4251,10 @@
         <v>127</v>
       </c>
       <c r="F98" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G98" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -4286,7 +4277,7 @@
         <v>302</v>
       </c>
       <c r="G99" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -4306,10 +4297,10 @@
         <v>129</v>
       </c>
       <c r="F100" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G100" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -4332,7 +4323,7 @@
         <v>277</v>
       </c>
       <c r="G101" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -4352,10 +4343,10 @@
         <v>131</v>
       </c>
       <c r="F102" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G102" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -4378,7 +4369,7 @@
         <v>291</v>
       </c>
       <c r="G103" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -4401,7 +4392,7 @@
         <v>298</v>
       </c>
       <c r="G104" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -4424,7 +4415,7 @@
         <v>280</v>
       </c>
       <c r="G105" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -4444,10 +4435,10 @@
         <v>133</v>
       </c>
       <c r="F106" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G106" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -4470,7 +4461,7 @@
         <v>283</v>
       </c>
       <c r="G107" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -4490,10 +4481,10 @@
         <v>135</v>
       </c>
       <c r="F108" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G108" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -4513,10 +4504,10 @@
         <v>136</v>
       </c>
       <c r="F109" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G109" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -4536,10 +4527,10 @@
         <v>137</v>
       </c>
       <c r="F110" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G110" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -4559,10 +4550,10 @@
         <v>138</v>
       </c>
       <c r="F111" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G111" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -4582,10 +4573,10 @@
         <v>139</v>
       </c>
       <c r="F112" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G112" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -4605,10 +4596,10 @@
         <v>140</v>
       </c>
       <c r="F113" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G113" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -4628,10 +4619,10 @@
         <v>141</v>
       </c>
       <c r="F114" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G114" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -4651,10 +4642,10 @@
         <v>142</v>
       </c>
       <c r="F115" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G115" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -4674,10 +4665,10 @@
         <v>143</v>
       </c>
       <c r="F116" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G116" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -4700,7 +4691,7 @@
         <v>289</v>
       </c>
       <c r="G117" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -4723,7 +4714,7 @@
         <v>290</v>
       </c>
       <c r="G118" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -4743,10 +4734,10 @@
         <v>142</v>
       </c>
       <c r="F119" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G119" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -4766,10 +4757,10 @@
         <v>146</v>
       </c>
       <c r="F120" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G120" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -4789,10 +4780,10 @@
         <v>147</v>
       </c>
       <c r="F121" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G121" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -4812,10 +4803,10 @@
         <v>148</v>
       </c>
       <c r="F122" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G122" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -4838,7 +4829,7 @@
         <v>290</v>
       </c>
       <c r="G123" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -4861,7 +4852,7 @@
         <v>290</v>
       </c>
       <c r="G124" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -4884,7 +4875,7 @@
         <v>289</v>
       </c>
       <c r="G125" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -4907,7 +4898,7 @@
         <v>309</v>
       </c>
       <c r="G126" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -4930,7 +4921,7 @@
         <v>283</v>
       </c>
       <c r="G127" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -4950,10 +4941,10 @@
         <v>153</v>
       </c>
       <c r="F128" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G128" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -4976,7 +4967,7 @@
         <v>283</v>
       </c>
       <c r="G129" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -4999,7 +4990,7 @@
         <v>289</v>
       </c>
       <c r="G130" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -5019,10 +5010,10 @@
         <v>156</v>
       </c>
       <c r="F131" t="s">
-        <v>331</v>
+        <v>281</v>
       </c>
       <c r="G131" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -5042,10 +5033,10 @@
         <v>157</v>
       </c>
       <c r="F132" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G132" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -5065,10 +5056,10 @@
         <v>158</v>
       </c>
       <c r="F133" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G133" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -5091,7 +5082,7 @@
         <v>290</v>
       </c>
       <c r="G134" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -5111,10 +5102,10 @@
         <v>160</v>
       </c>
       <c r="F135" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G135" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -5137,7 +5128,7 @@
         <v>289</v>
       </c>
       <c r="G136" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -5157,10 +5148,10 @@
         <v>162</v>
       </c>
       <c r="F137" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G137" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -5183,7 +5174,7 @@
         <v>290</v>
       </c>
       <c r="G138" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -5206,7 +5197,7 @@
         <v>290</v>
       </c>
       <c r="G139" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -5226,10 +5217,10 @@
         <v>165</v>
       </c>
       <c r="F140" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G140" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -5249,10 +5240,10 @@
         <v>166</v>
       </c>
       <c r="F141" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G141" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -5275,7 +5266,7 @@
         <v>309</v>
       </c>
       <c r="G142" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -5295,10 +5286,10 @@
         <v>168</v>
       </c>
       <c r="F143" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G143" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="144" spans="1:7">
@@ -5321,7 +5312,7 @@
         <v>283</v>
       </c>
       <c r="G144" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="145" spans="1:7">
@@ -5344,7 +5335,7 @@
         <v>283</v>
       </c>
       <c r="G145" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="146" spans="1:7">
@@ -5364,10 +5355,10 @@
         <v>170</v>
       </c>
       <c r="F146" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G146" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="147" spans="1:7">
@@ -5387,10 +5378,10 @@
         <v>171</v>
       </c>
       <c r="F147" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G147" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="148" spans="1:7">
@@ -5410,10 +5401,10 @@
         <v>172</v>
       </c>
       <c r="F148" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G148" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="149" spans="1:7">
@@ -5433,10 +5424,10 @@
         <v>173</v>
       </c>
       <c r="F149" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G149" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="150" spans="1:7">
@@ -5459,7 +5450,7 @@
         <v>283</v>
       </c>
       <c r="G150" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="151" spans="1:7">
@@ -5482,7 +5473,7 @@
         <v>283</v>
       </c>
       <c r="G151" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="152" spans="1:7">
@@ -5505,7 +5496,7 @@
         <v>290</v>
       </c>
       <c r="G152" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -5528,7 +5519,7 @@
         <v>283</v>
       </c>
       <c r="G153" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -5551,7 +5542,7 @@
         <v>283</v>
       </c>
       <c r="G154" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="155" spans="1:7">
@@ -5571,10 +5562,10 @@
         <v>179</v>
       </c>
       <c r="F155" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G155" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="156" spans="1:7">
@@ -5597,7 +5588,7 @@
         <v>309</v>
       </c>
       <c r="G156" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="157" spans="1:7">
@@ -5617,10 +5608,10 @@
         <v>181</v>
       </c>
       <c r="F157" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G157" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="158" spans="1:7">
@@ -5643,7 +5634,7 @@
         <v>309</v>
       </c>
       <c r="G158" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="159" spans="1:7">
@@ -5663,10 +5654,10 @@
         <v>183</v>
       </c>
       <c r="F159" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G159" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="160" spans="1:7">
@@ -5686,10 +5677,10 @@
         <v>184</v>
       </c>
       <c r="F160" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G160" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="161" spans="1:7">
@@ -5709,10 +5700,10 @@
         <v>142</v>
       </c>
       <c r="F161" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G161" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="162" spans="1:7">
@@ -5732,10 +5723,10 @@
         <v>185</v>
       </c>
       <c r="F162" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G162" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="163" spans="1:7">
@@ -5755,10 +5746,10 @@
         <v>186</v>
       </c>
       <c r="F163" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G163" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="164" spans="1:7">
@@ -5778,10 +5769,10 @@
         <v>187</v>
       </c>
       <c r="F164" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G164" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="165" spans="1:7">
@@ -5801,10 +5792,10 @@
         <v>188</v>
       </c>
       <c r="F165" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G165" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="166" spans="1:7">
@@ -5827,7 +5818,7 @@
         <v>290</v>
       </c>
       <c r="G166" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="167" spans="1:7">
@@ -5847,10 +5838,10 @@
         <v>142</v>
       </c>
       <c r="F167" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G167" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="168" spans="1:7">
@@ -5870,10 +5861,10 @@
         <v>190</v>
       </c>
       <c r="F168" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G168" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="169" spans="1:7">
@@ -5893,10 +5884,10 @@
         <v>191</v>
       </c>
       <c r="F169" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G169" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="170" spans="1:7">
@@ -5919,7 +5910,7 @@
         <v>283</v>
       </c>
       <c r="G170" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="171" spans="1:7">
@@ -5942,7 +5933,7 @@
         <v>283</v>
       </c>
       <c r="G171" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="172" spans="1:7">
@@ -5962,10 +5953,10 @@
         <v>194</v>
       </c>
       <c r="F172" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G172" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="173" spans="1:7">
@@ -5985,10 +5976,10 @@
         <v>142</v>
       </c>
       <c r="F173" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G173" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="174" spans="1:7">
@@ -6008,10 +5999,10 @@
         <v>195</v>
       </c>
       <c r="F174" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G174" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="175" spans="1:7">
@@ -6031,10 +6022,10 @@
         <v>196</v>
       </c>
       <c r="F175" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G175" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="176" spans="1:7">
@@ -6057,7 +6048,7 @@
         <v>309</v>
       </c>
       <c r="G176" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="177" spans="1:7">
@@ -6077,10 +6068,10 @@
         <v>198</v>
       </c>
       <c r="F177" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G177" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="178" spans="1:7">
@@ -6103,7 +6094,7 @@
         <v>304</v>
       </c>
       <c r="G178" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="179" spans="1:7">
@@ -6126,7 +6117,7 @@
         <v>283</v>
       </c>
       <c r="G179" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="180" spans="1:7">
@@ -6146,10 +6137,10 @@
         <v>201</v>
       </c>
       <c r="F180" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G180" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="181" spans="1:7">
@@ -6169,10 +6160,10 @@
         <v>202</v>
       </c>
       <c r="F181" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G181" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="182" spans="1:7">
@@ -6195,7 +6186,7 @@
         <v>283</v>
       </c>
       <c r="G182" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="183" spans="1:7">
@@ -6215,10 +6206,10 @@
         <v>204</v>
       </c>
       <c r="F183" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G183" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="184" spans="1:7">
@@ -6241,7 +6232,7 @@
         <v>309</v>
       </c>
       <c r="G184" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="185" spans="1:7">
@@ -6261,10 +6252,10 @@
         <v>206</v>
       </c>
       <c r="F185" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G185" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="186" spans="1:7">
@@ -6287,7 +6278,7 @@
         <v>309</v>
       </c>
       <c r="G186" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="187" spans="1:7">
@@ -6310,7 +6301,7 @@
         <v>290</v>
       </c>
       <c r="G187" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="188" spans="1:7">
@@ -6333,7 +6324,7 @@
         <v>283</v>
       </c>
       <c r="G188" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="189" spans="1:7">
@@ -6356,7 +6347,7 @@
         <v>283</v>
       </c>
       <c r="G189" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="190" spans="1:7">
@@ -6376,10 +6367,10 @@
         <v>210</v>
       </c>
       <c r="F190" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G190" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="191" spans="1:7">
@@ -6399,10 +6390,10 @@
         <v>198</v>
       </c>
       <c r="F191" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G191" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="192" spans="1:7">
@@ -6425,7 +6416,7 @@
         <v>290</v>
       </c>
       <c r="G192" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="193" spans="1:7">
@@ -6445,10 +6436,10 @@
         <v>142</v>
       </c>
       <c r="F193" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G193" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="194" spans="1:7">
@@ -6471,7 +6462,7 @@
         <v>290</v>
       </c>
       <c r="G194" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="195" spans="1:7">
@@ -6491,10 +6482,10 @@
         <v>213</v>
       </c>
       <c r="F195" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G195" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="196" spans="1:7">
@@ -6514,10 +6505,10 @@
         <v>214</v>
       </c>
       <c r="F196" t="s">
-        <v>347</v>
+        <v>287</v>
       </c>
       <c r="G196" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="197" spans="1:7">
@@ -6540,7 +6531,7 @@
         <v>277</v>
       </c>
       <c r="G197" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="198" spans="1:7">
@@ -6560,10 +6551,10 @@
         <v>215</v>
       </c>
       <c r="F198" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G198" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="199" spans="1:7">
@@ -6586,7 +6577,7 @@
         <v>289</v>
       </c>
       <c r="G199" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="200" spans="1:7">
@@ -6609,7 +6600,7 @@
         <v>304</v>
       </c>
       <c r="G200" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="201" spans="1:7">
@@ -6629,10 +6620,10 @@
         <v>142</v>
       </c>
       <c r="F201" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G201" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="202" spans="1:7">
@@ -6655,7 +6646,7 @@
         <v>277</v>
       </c>
       <c r="G202" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="203" spans="1:7">
@@ -6678,7 +6669,7 @@
         <v>277</v>
       </c>
       <c r="G203" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="204" spans="1:7">
@@ -6698,10 +6689,10 @@
         <v>219</v>
       </c>
       <c r="F204" t="s">
-        <v>310</v>
+        <v>280</v>
       </c>
       <c r="G204" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="205" spans="1:7">
@@ -6721,10 +6712,10 @@
         <v>220</v>
       </c>
       <c r="F205" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G205" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="206" spans="1:7">
@@ -6747,7 +6738,7 @@
         <v>287</v>
       </c>
       <c r="G206" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="207" spans="1:7">
@@ -6767,10 +6758,10 @@
         <v>222</v>
       </c>
       <c r="F207" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G207" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="208" spans="1:7">
@@ -6793,7 +6784,7 @@
         <v>277</v>
       </c>
       <c r="G208" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="209" spans="1:7">
@@ -6813,10 +6804,10 @@
         <v>224</v>
       </c>
       <c r="F209" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G209" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="210" spans="1:7">
@@ -6839,7 +6830,7 @@
         <v>277</v>
       </c>
       <c r="G210" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="211" spans="1:7">
@@ -6859,10 +6850,10 @@
         <v>226</v>
       </c>
       <c r="F211" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G211" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="212" spans="1:7">
@@ -6882,10 +6873,10 @@
         <v>227</v>
       </c>
       <c r="F212" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G212" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="213" spans="1:7">
@@ -6908,7 +6899,7 @@
         <v>291</v>
       </c>
       <c r="G213" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="214" spans="1:7">
@@ -6931,7 +6922,7 @@
         <v>283</v>
       </c>
       <c r="G214" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="215" spans="1:7">
@@ -6954,7 +6945,7 @@
         <v>283</v>
       </c>
       <c r="G215" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="216" spans="1:7">
@@ -6974,10 +6965,10 @@
         <v>229</v>
       </c>
       <c r="F216" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G216" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="217" spans="1:7">
@@ -7000,7 +6991,7 @@
         <v>289</v>
       </c>
       <c r="G217" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="218" spans="1:7">
@@ -7020,10 +7011,10 @@
         <v>231</v>
       </c>
       <c r="F218" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G218" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="219" spans="1:7">
@@ -7046,7 +7037,7 @@
         <v>289</v>
       </c>
       <c r="G219" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="220" spans="1:7">
@@ -7069,7 +7060,7 @@
         <v>277</v>
       </c>
       <c r="G220" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="221" spans="1:7">
@@ -7092,7 +7083,7 @@
         <v>283</v>
       </c>
       <c r="G221" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="222" spans="1:7">
@@ -7115,7 +7106,7 @@
         <v>284</v>
       </c>
       <c r="G222" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="223" spans="1:7">
@@ -7135,10 +7126,10 @@
         <v>235</v>
       </c>
       <c r="F223" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G223" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="224" spans="1:7">
@@ -7158,10 +7149,10 @@
         <v>236</v>
       </c>
       <c r="F224" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G224" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="225" spans="1:7">
@@ -7181,10 +7172,10 @@
         <v>237</v>
       </c>
       <c r="F225" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G225" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="226" spans="1:7">
@@ -7207,7 +7198,7 @@
         <v>290</v>
       </c>
       <c r="G226" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="227" spans="1:7">
@@ -7227,10 +7218,10 @@
         <v>239</v>
       </c>
       <c r="F227" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="G227" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="228" spans="1:7">
@@ -7253,7 +7244,7 @@
         <v>283</v>
       </c>
       <c r="G228" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="229" spans="1:7">
@@ -7273,10 +7264,10 @@
         <v>241</v>
       </c>
       <c r="F229" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G229" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="230" spans="1:7">
@@ -7299,7 +7290,7 @@
         <v>290</v>
       </c>
       <c r="G230" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="231" spans="1:7">
@@ -7319,10 +7310,10 @@
         <v>243</v>
       </c>
       <c r="F231" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="G231" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="232" spans="1:7">
@@ -7345,7 +7336,7 @@
         <v>283</v>
       </c>
       <c r="G232" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="233" spans="1:7">
@@ -7365,10 +7356,10 @@
         <v>179</v>
       </c>
       <c r="F233" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G233" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="234" spans="1:7">
@@ -7388,10 +7379,10 @@
         <v>245</v>
       </c>
       <c r="F234" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G234" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="235" spans="1:7">
@@ -7411,10 +7402,10 @@
         <v>246</v>
       </c>
       <c r="F235" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="G235" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="236" spans="1:7">
@@ -7437,7 +7428,7 @@
         <v>304</v>
       </c>
       <c r="G236" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="237" spans="1:7">
@@ -7460,7 +7451,7 @@
         <v>290</v>
       </c>
       <c r="G237" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="238" spans="1:7">
@@ -7483,7 +7474,7 @@
         <v>309</v>
       </c>
       <c r="G238" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="239" spans="1:7">
@@ -7503,10 +7494,10 @@
         <v>249</v>
       </c>
       <c r="F239" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G239" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="240" spans="1:7">
@@ -7529,7 +7520,7 @@
         <v>287</v>
       </c>
       <c r="G240" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="241" spans="1:7">
@@ -7552,7 +7543,7 @@
         <v>277</v>
       </c>
       <c r="G241" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="242" spans="1:7">
@@ -7572,10 +7563,10 @@
         <v>251</v>
       </c>
       <c r="F242" t="s">
-        <v>347</v>
+        <v>287</v>
       </c>
       <c r="G242" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="243" spans="1:7">
@@ -7598,7 +7589,7 @@
         <v>302</v>
       </c>
       <c r="G243" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="244" spans="1:7">
@@ -7618,10 +7609,10 @@
         <v>252</v>
       </c>
       <c r="F244" t="s">
-        <v>310</v>
+        <v>280</v>
       </c>
       <c r="G244" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="245" spans="1:7">
@@ -7644,7 +7635,7 @@
         <v>280</v>
       </c>
       <c r="G245" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="246" spans="1:7">
@@ -7667,7 +7658,7 @@
         <v>290</v>
       </c>
       <c r="G246" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="247" spans="1:7">
@@ -7687,10 +7678,10 @@
         <v>255</v>
       </c>
       <c r="F247" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G247" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="248" spans="1:7">
@@ -7713,7 +7704,7 @@
         <v>284</v>
       </c>
       <c r="G248" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="249" spans="1:7">
@@ -7733,10 +7724,10 @@
         <v>257</v>
       </c>
       <c r="F249" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="G249" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="250" spans="1:7">
@@ -7759,7 +7750,7 @@
         <v>293</v>
       </c>
       <c r="G250" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="251" spans="1:7">
@@ -7782,7 +7773,7 @@
         <v>293</v>
       </c>
       <c r="G251" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="252" spans="1:7">
@@ -7805,7 +7796,7 @@
         <v>277</v>
       </c>
       <c r="G252" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="253" spans="1:7">
@@ -7828,7 +7819,7 @@
         <v>277</v>
       </c>
       <c r="G253" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="254" spans="1:7">
@@ -7848,10 +7839,10 @@
         <v>261</v>
       </c>
       <c r="F254" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="G254" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="255" spans="1:7">
@@ -7871,10 +7862,10 @@
         <v>262</v>
       </c>
       <c r="F255" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="G255" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="256" spans="1:7">
@@ -7894,10 +7885,10 @@
         <v>263</v>
       </c>
       <c r="F256" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G256" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="257" spans="1:7">
@@ -7917,10 +7908,10 @@
         <v>264</v>
       </c>
       <c r="F257" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G257" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="258" spans="1:7">
@@ -7943,7 +7934,7 @@
         <v>283</v>
       </c>
       <c r="G258" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="259" spans="1:7">
@@ -7966,7 +7957,7 @@
         <v>283</v>
       </c>
       <c r="G259" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="260" spans="1:7">
@@ -7989,7 +7980,7 @@
         <v>283</v>
       </c>
       <c r="G260" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="261" spans="1:7">
@@ -8012,7 +8003,7 @@
         <v>283</v>
       </c>
       <c r="G261" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="262" spans="1:7">
@@ -8035,7 +8026,7 @@
         <v>290</v>
       </c>
       <c r="G262" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="263" spans="1:7">
@@ -8055,10 +8046,10 @@
         <v>235</v>
       </c>
       <c r="F263" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G263" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="264" spans="1:7">
@@ -8081,7 +8072,7 @@
         <v>290</v>
       </c>
       <c r="G264" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="265" spans="1:7">
@@ -8101,10 +8092,10 @@
         <v>270</v>
       </c>
       <c r="F265" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G265" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="266" spans="1:7">
@@ -8124,10 +8115,10 @@
         <v>271</v>
       </c>
       <c r="F266" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G266" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="267" spans="1:7">
@@ -8147,10 +8138,10 @@
         <v>272</v>
       </c>
       <c r="F267" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G267" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="268" spans="1:7">
@@ -8173,7 +8164,7 @@
         <v>283</v>
       </c>
       <c r="G268" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="269" spans="1:7">
@@ -8193,10 +8184,10 @@
         <v>274</v>
       </c>
       <c r="F269" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G269" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="270" spans="1:7">
@@ -8219,7 +8210,7 @@
         <v>290</v>
       </c>
       <c r="G270" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="271" spans="1:7">
@@ -8239,10 +8230,10 @@
         <v>276</v>
       </c>
       <c r="F271" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G271" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>

</xml_diff>